<commit_message>
Add the install & uninstall app test cases
</commit_message>
<xml_diff>
--- a/TestData/temp_email_mca.xlsx
+++ b/TestData/temp_email_mca.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
   <si>
     <t>Email</t>
   </si>
@@ -72,6 +72,129 @@
   </si>
   <si>
     <t>usx34296@nezid.com</t>
+  </si>
+  <si>
+    <t>tur94607@nezid.com</t>
+  </si>
+  <si>
+    <t>bre36090@nezid.com</t>
+  </si>
+  <si>
+    <t>tur93409@zslsz.com</t>
+  </si>
+  <si>
+    <t>fao95745@zslsz.com</t>
+  </si>
+  <si>
+    <t>ruh49712@omeie.com</t>
+  </si>
+  <si>
+    <t>tjl35368@nezid.com</t>
+  </si>
+  <si>
+    <t>xou82046@omeie.com</t>
+  </si>
+  <si>
+    <t>hof34724@zbock.com</t>
+  </si>
+  <si>
+    <t>lgv54003@zbock.com</t>
+  </si>
+  <si>
+    <t>lre70178@zbock.com</t>
+  </si>
+  <si>
+    <t>xem17292@omeie.com</t>
+  </si>
+  <si>
+    <t>pow81042@nezid.com</t>
+  </si>
+  <si>
+    <t>znq06487@nezid.com</t>
+  </si>
+  <si>
+    <t>dkf37754@omeie.com</t>
+  </si>
+  <si>
+    <t>fbe47753@omeie.com</t>
+  </si>
+  <si>
+    <t>amw61396@zbock.com</t>
+  </si>
+  <si>
+    <t>hcj03458@nezid.com</t>
+  </si>
+  <si>
+    <t>rzo03459@omeie.com</t>
+  </si>
+  <si>
+    <t>rhf07378@nezid.com</t>
+  </si>
+  <si>
+    <t>aez44973@zslsz.com</t>
+  </si>
+  <si>
+    <t>wbn31967@zslsz.com</t>
+  </si>
+  <si>
+    <t>akv81094@omeie.com</t>
+  </si>
+  <si>
+    <t>wqo14692@zslsz.com</t>
+  </si>
+  <si>
+    <t>pqt08842@zbock.com</t>
+  </si>
+  <si>
+    <t>aht64573@nezid.com</t>
+  </si>
+  <si>
+    <t>tjc10801@zslsz.com</t>
+  </si>
+  <si>
+    <t>fip11442@zbock.com</t>
+  </si>
+  <si>
+    <t>qck02640@zslsz.com</t>
+  </si>
+  <si>
+    <t>cwm75412@zslsz.com</t>
+  </si>
+  <si>
+    <t>jog92534@zbock.com</t>
+  </si>
+  <si>
+    <t>ksi89017@omeie.com</t>
+  </si>
+  <si>
+    <t>ybp81275@zslsz.com</t>
+  </si>
+  <si>
+    <t>mlf16659@omeie.com</t>
+  </si>
+  <si>
+    <t>oso98765@nezid.com</t>
+  </si>
+  <si>
+    <t>yia52446@nezid.com</t>
+  </si>
+  <si>
+    <t>oxm17594@zslsz.com</t>
+  </si>
+  <si>
+    <t>ncy71978@zbock.com</t>
+  </si>
+  <si>
+    <t>epa69634@nezid.com</t>
+  </si>
+  <si>
+    <t>zmr75255@nezid.com</t>
+  </si>
+  <si>
+    <t>ude61198@omeie.com</t>
+  </si>
+  <si>
+    <t>qsa66922@nezid.com</t>
   </si>
 </sst>
 </file>
@@ -116,7 +239,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -217,6 +340,211 @@
         <v>19</v>
       </c>
     </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Update creating order test cases and add test case for getting summary report
</commit_message>
<xml_diff>
--- a/TestData/temp_email_mca.xlsx
+++ b/TestData/temp_email_mca.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="80">
   <si>
     <t>Email</t>
   </si>
@@ -195,6 +195,63 @@
   </si>
   <si>
     <t>qsa66922@nezid.com</t>
+  </si>
+  <si>
+    <t>ikk58050@zbock.com</t>
+  </si>
+  <si>
+    <t>sns62539@zbock.com</t>
+  </si>
+  <si>
+    <t>ool45473@omeie.com</t>
+  </si>
+  <si>
+    <t>csz39978@nezid.com</t>
+  </si>
+  <si>
+    <t>obo64382@omeie.com</t>
+  </si>
+  <si>
+    <t>ssv86936@zbock.com</t>
+  </si>
+  <si>
+    <t>abg80663@zbock.com</t>
+  </si>
+  <si>
+    <t>uzm01189@zslsz.com</t>
+  </si>
+  <si>
+    <t>xif30473@omeie.com</t>
+  </si>
+  <si>
+    <t>klz21931@nezid.com</t>
+  </si>
+  <si>
+    <t>gza24518@omeie.com</t>
+  </si>
+  <si>
+    <t>tzl06814@nezid.com</t>
+  </si>
+  <si>
+    <t>qky16640@zslsz.com</t>
+  </si>
+  <si>
+    <t>hko75455@omeie.com</t>
+  </si>
+  <si>
+    <t>spq38435@zbock.com</t>
+  </si>
+  <si>
+    <t>icy48459@zbock.com</t>
+  </si>
+  <si>
+    <t>dcn67384@zbock.com</t>
+  </si>
+  <si>
+    <t>ywd16426@omeie.com</t>
+  </si>
+  <si>
+    <t>awa67260@nezid.com</t>
   </si>
 </sst>
 </file>
@@ -239,7 +296,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B60"/>
+  <dimension ref="A1:B79"/>
   <sheetViews>
     <sheetView tabSelected="true" workbookViewId="0"/>
   </sheetViews>
@@ -545,6 +602,101 @@
         <v>60</v>
       </c>
     </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>